<commit_message>
orden de las carpetas de admin y uniones
</commit_message>
<xml_diff>
--- a/bd/pedidos.xlsx
+++ b/bd/pedidos.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,22 +422,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>id_pedido</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>id_usuario</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>fecha_pedido</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>estado</t>
         </is>
@@ -471,7 +459,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>pagado</t>
+          <t>enviado</t>
         </is>
       </c>
     </row>

</xml_diff>